<commit_message>
Updated readme  and completed tests.
</commit_message>
<xml_diff>
--- a/raw_module_data/CEC/Battery_List.xlsx
+++ b/raw_module_data/CEC/Battery_List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djp12\Documents\Coding\Github_Repos\WiseWattage\data\CEC_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djp12\Documents\Coding\Github_Repos\WiseWattage\raw_module_data\CEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CA0E18-2D9B-4E5D-BE88-25F23579BB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10731674-33CE-43B1-87EE-C386EDF13EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25955,26 +25955,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5067c814-4b34-462c-a21d-c185ff6548d2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="785685f2-c2e1-4352-89aa-3faca8eaba52">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010061DC9A153AAEEE45BACE06E01F8272AC" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4090c5de22bf8b351fb71f0d3285de4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="785685f2-c2e1-4352-89aa-3faca8eaba52" xmlns:ns3="5067c814-4b34-462c-a21d-c185ff6548d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64236aafc598cdb45171e1885433f021" ns2:_="" ns3:_="">
     <xsd:import namespace="785685f2-c2e1-4352-89aa-3faca8eaba52"/>
@@ -26209,10 +26189,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5067c814-4b34-462c-a21d-c185ff6548d2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="785685f2-c2e1-4352-89aa-3faca8eaba52">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DCFC1B5-7558-469A-9701-49121208929A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AD4E4C8-2654-4D95-B6F5-79842D2E8A6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="785685f2-c2e1-4352-89aa-3faca8eaba52"/>
+    <ds:schemaRef ds:uri="5067c814-4b34-462c-a21d-c185ff6548d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26235,20 +26246,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AD4E4C8-2654-4D95-B6F5-79842D2E8A6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DCFC1B5-7558-469A-9701-49121208929A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="785685f2-c2e1-4352-89aa-3faca8eaba52"/>
-    <ds:schemaRef ds:uri="5067c814-4b34-462c-a21d-c185ff6548d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>